<commit_message>
add order in horarios
</commit_message>
<xml_diff>
--- a/assets/templates/Teorico para aula MODELO.xlsx
+++ b/assets/templates/Teorico para aula MODELO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60990B74-B3F0-4E9A-9F36-245001668604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE65CDF-50F7-4690-BD39-7BCC701E6410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="1380" windowWidth="21600" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -639,6 +639,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1065,8 +1069,8 @@
   </sheetPr>
   <dimension ref="A1:AJ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2307,7 +2311,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
+      <c r="M30" s="74"/>
       <c r="N30" s="41"/>
       <c r="O30" s="41"/>
       <c r="P30" s="42"/>
@@ -2348,7 +2352,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
+      <c r="M31" s="37"/>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
       <c r="P31" s="36"/>
@@ -2390,7 +2394,7 @@
       <c r="K32" s="34"/>
       <c r="L32" s="34"/>
       <c r="M32" s="35"/>
-      <c r="N32" s="37"/>
+      <c r="N32" s="34"/>
       <c r="O32" s="34"/>
       <c r="P32" s="36"/>
       <c r="Q32" s="21"/>
@@ -2431,7 +2435,7 @@
       <c r="K33" s="34"/>
       <c r="L33" s="34"/>
       <c r="M33" s="35"/>
-      <c r="N33" s="37"/>
+      <c r="N33" s="34"/>
       <c r="O33" s="34"/>
       <c r="P33" s="36"/>
       <c r="Q33" s="21"/>
@@ -2472,7 +2476,7 @@
       <c r="K34" s="34"/>
       <c r="L34" s="34"/>
       <c r="M34" s="35"/>
-      <c r="N34" s="37"/>
+      <c r="N34" s="34"/>
       <c r="O34" s="34"/>
       <c r="P34" s="36"/>
       <c r="Q34" s="21"/>
@@ -2513,7 +2517,7 @@
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
       <c r="M35" s="35"/>
-      <c r="N35" s="37"/>
+      <c r="N35" s="34"/>
       <c r="O35" s="34"/>
       <c r="P35" s="36"/>
       <c r="Q35" s="21"/>
@@ -2554,7 +2558,7 @@
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
       <c r="M36" s="35"/>
-      <c r="N36" s="37"/>
+      <c r="N36" s="34"/>
       <c r="O36" s="34"/>
       <c r="P36" s="36"/>
       <c r="Q36" s="21"/>
@@ -2595,7 +2599,7 @@
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
       <c r="M37" s="35"/>
-      <c r="N37" s="37"/>
+      <c r="N37" s="34"/>
       <c r="O37" s="34"/>
       <c r="P37" s="36"/>
       <c r="Q37" s="21"/>
@@ -2636,7 +2640,7 @@
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
       <c r="M38" s="35"/>
-      <c r="N38" s="37"/>
+      <c r="N38" s="34"/>
       <c r="O38" s="34"/>
       <c r="P38" s="36"/>
       <c r="Q38" s="21"/>
@@ -2677,7 +2681,7 @@
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="35"/>
-      <c r="N39" s="37"/>
+      <c r="N39" s="34"/>
       <c r="O39" s="34"/>
       <c r="P39" s="36"/>
       <c r="Q39" s="21"/>
@@ -2718,7 +2722,7 @@
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="35"/>
-      <c r="N40" s="37"/>
+      <c r="N40" s="34"/>
       <c r="O40" s="34"/>
       <c r="P40" s="36"/>
       <c r="Q40" s="21"/>
@@ -2759,7 +2763,7 @@
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
       <c r="M41" s="35"/>
-      <c r="N41" s="37"/>
+      <c r="N41" s="34"/>
       <c r="O41" s="34"/>
       <c r="P41" s="36"/>
       <c r="Q41" s="21"/>
@@ -2800,7 +2804,7 @@
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="35"/>
-      <c r="N42" s="37"/>
+      <c r="N42" s="34"/>
       <c r="O42" s="49"/>
       <c r="P42" s="36"/>
       <c r="Q42" s="21"/>
@@ -2841,7 +2845,7 @@
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
       <c r="M43" s="35"/>
-      <c r="N43" s="37"/>
+      <c r="N43" s="34"/>
       <c r="O43" s="34"/>
       <c r="P43" s="36"/>
       <c r="Q43" s="25"/>

</xml_diff>